<commit_message>
Proper sorting of the constraing aliases
</commit_message>
<xml_diff>
--- a/apricot-reports/ApricotIntermediaryAgreementReport.xlsx
+++ b/apricot-reports/ApricotIntermediaryAgreementReport.xlsx
@@ -371,15 +371,15 @@
     <t>intermediary_agreement_id *</t>
   </si>
   <si>
+    <t>FK1</t>
+  </si>
+  <si>
+    <t>redirect_to_id</t>
+  </si>
+  <si>
     <t>FK2</t>
   </si>
   <si>
-    <t>redirect_to_id</t>
-  </si>
-  <si>
-    <t>FK1</t>
-  </si>
-  <si>
     <t>smallint</t>
   </si>
   <si>
@@ -503,7 +503,7 @@
     <t>contract_component_id *</t>
   </si>
   <si>
-    <t>FK, IDX1</t>
+    <t>FK, IDX</t>
   </si>
   <si>
     <t>attribute_name *</t>
@@ -605,81 +605,81 @@
     <t>title_id *</t>
   </si>
   <si>
+    <t>mis_role</t>
+  </si>
+  <si>
+    <t>reserve_specification</t>
+  </si>
+  <si>
+    <t>default_reserve_id</t>
+  </si>
+  <si>
+    <t>FK3</t>
+  </si>
+  <si>
+    <t>relationship_specification</t>
+  </si>
+  <si>
+    <t>payment_specification_id</t>
+  </si>
+  <si>
+    <t>fsb_registration_specification</t>
+  </si>
+  <si>
+    <t>fsb_registration_specification_id</t>
+  </si>
+  <si>
+    <t>FK4</t>
+  </si>
+  <si>
+    <t>contract_specification_product_category</t>
+  </si>
+  <si>
+    <t>party_type</t>
+  </si>
+  <si>
+    <t>rem_stmnt_tmpl_cat_id</t>
+  </si>
+  <si>
+    <t>FK5</t>
+  </si>
+  <si>
+    <t>default_open_for_new_business</t>
+  </si>
+  <si>
+    <t>open_for_new_business_editable</t>
+  </si>
+  <si>
+    <t>organisation_manager</t>
+  </si>
+  <si>
+    <t>sub_status_specification</t>
+  </si>
+  <si>
+    <t>sub_status_specification_id</t>
+  </si>
+  <si>
     <t>FK6</t>
   </si>
   <si>
-    <t>mis_role</t>
-  </si>
-  <si>
-    <t>reserve_specification</t>
-  </si>
-  <si>
-    <t>default_reserve_id</t>
-  </si>
-  <si>
-    <t>relationship_specification</t>
-  </si>
-  <si>
-    <t>payment_specification_id</t>
-  </si>
-  <si>
-    <t>fsb_registration_specification</t>
-  </si>
-  <si>
-    <t>fsb_registration_specification_id</t>
-  </si>
-  <si>
-    <t>FK3</t>
-  </si>
-  <si>
-    <t>contract_specification_product_category</t>
-  </si>
-  <si>
-    <t>party_type</t>
-  </si>
-  <si>
-    <t>rem_stmnt_tmpl_cat_id</t>
+    <t>termination_reason_specification</t>
+  </si>
+  <si>
+    <t>termination_reason_specification_id</t>
+  </si>
+  <si>
+    <t>FK7</t>
+  </si>
+  <si>
+    <t>graduation_phase</t>
+  </si>
+  <si>
+    <t>default_graduation_phase_id</t>
   </si>
   <si>
     <t>FK8</t>
   </si>
   <si>
-    <t>default_open_for_new_business</t>
-  </si>
-  <si>
-    <t>open_for_new_business_editable</t>
-  </si>
-  <si>
-    <t>organisation_manager</t>
-  </si>
-  <si>
-    <t>sub_status_specification</t>
-  </si>
-  <si>
-    <t>sub_status_specification_id</t>
-  </si>
-  <si>
-    <t>FK4</t>
-  </si>
-  <si>
-    <t>termination_reason_specification</t>
-  </si>
-  <si>
-    <t>termination_reason_specification_id</t>
-  </si>
-  <si>
-    <t>FK5</t>
-  </si>
-  <si>
-    <t>graduation_phase</t>
-  </si>
-  <si>
-    <t>default_graduation_phase_id</t>
-  </si>
-  <si>
-    <t>FK7</t>
-  </si>
-  <si>
     <t>sign_away_rights_enabled</t>
   </si>
   <si>
@@ -878,7 +878,7 @@
     <t>date_of_commencement</t>
   </si>
   <si>
-    <t>FK2, IDX</t>
+    <t>FK1, IDX</t>
   </si>
   <si>
     <t>intermediary_reserve_data</t>
@@ -887,7 +887,7 @@
     <t>reserve_data_id</t>
   </si>
   <si>
-    <t>FK5, FK9</t>
+    <t>FK2, FK3</t>
   </si>
   <si>
     <t>date_of_termination</t>
@@ -902,60 +902,66 @@
     <t>termination_reason_primary_id</t>
   </si>
   <si>
+    <t>termination_reason_secondary_id</t>
+  </si>
+  <si>
+    <t>FK5, FK6</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>sub_status</t>
+  </si>
+  <si>
+    <t>reappointment_not_recommended</t>
+  </si>
+  <si>
+    <t>intermediary_agreement_commission_split</t>
+  </si>
+  <si>
+    <t>possible_debarment</t>
+  </si>
+  <si>
+    <t>open_for_new_business</t>
+  </si>
+  <si>
+    <t>open_for_financing</t>
+  </si>
+  <si>
+    <t>fica_compliance_id</t>
+  </si>
+  <si>
+    <t>FK7, FK8</t>
+  </si>
+  <si>
+    <t>termination_transaction_date</t>
+  </si>
+  <si>
+    <t>termination_timestamp</t>
+  </si>
+  <si>
+    <t>service_months_id</t>
+  </si>
+  <si>
+    <t>FK9</t>
+  </si>
+  <si>
+    <t>FK10</t>
+  </si>
+  <si>
+    <t>parent_entity_id</t>
+  </si>
+  <si>
+    <t>FK11</t>
+  </si>
+  <si>
+    <t>proof_of_intent_to</t>
+  </si>
+  <si>
     <t>FK12</t>
   </si>
   <si>
-    <t>termination_reason_secondary_id</t>
-  </si>
-  <si>
-    <t>FK11, FK13</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>sub_status</t>
-  </si>
-  <si>
-    <t>reappointment_not_recommended</t>
-  </si>
-  <si>
-    <t>intermediary_agreement_commission_split</t>
-  </si>
-  <si>
-    <t>possible_debarment</t>
-  </si>
-  <si>
-    <t>open_for_new_business</t>
-  </si>
-  <si>
-    <t>open_for_financing</t>
-  </si>
-  <si>
-    <t>fica_compliance_id</t>
-  </si>
-  <si>
-    <t>FK3, FK4</t>
-  </si>
-  <si>
-    <t>termination_transaction_date</t>
-  </si>
-  <si>
-    <t>termination_timestamp</t>
-  </si>
-  <si>
-    <t>service_months_id</t>
-  </si>
-  <si>
-    <t>FK10</t>
-  </si>
-  <si>
-    <t>parent_entity_id</t>
-  </si>
-  <si>
-    <t>proof_of_intent_to</t>
-  </si>
-  <si>
     <t>sign_away_rights</t>
   </si>
   <si>
@@ -983,6 +989,9 @@
     <t>redirect_balance_intermediary_agreement_id</t>
   </si>
   <si>
+    <t>FK13</t>
+  </si>
+  <si>
     <t>redirect_balance_type_id</t>
   </si>
   <si>
@@ -1004,21 +1013,15 @@
     <t>intermediary_agreement_nub_reason</t>
   </si>
   <si>
+    <t>agreement_warning_id *</t>
+  </si>
+  <si>
     <t>PK, FK2, FK3</t>
   </si>
   <si>
-    <t>agreement_warning_id *</t>
-  </si>
-  <si>
     <t>contract_component_attribute_id *</t>
   </si>
   <si>
-    <t>FK, IDX</t>
-  </si>
-  <si>
-    <t>FK1, IDX</t>
-  </si>
-  <si>
     <t>component_active</t>
   </si>
   <si>
@@ -1073,16 +1076,13 @@
     <t>agreement_id *</t>
   </si>
   <si>
-    <t>FK, IDX1, IDX2</t>
+    <t>FK, IDX, IDX1</t>
   </si>
   <si>
     <t>IDX, IDX1, IDX2</t>
   </si>
   <si>
     <t>party_role_type</t>
-  </si>
-  <si>
-    <t>IDX1</t>
   </si>
   <si>
     <t>historic_linking_group_id</t>
@@ -4652,7 +4652,7 @@
         <v>8</v>
       </c>
       <c r="E152" t="s" s="133">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F152" s="133"/>
     </row>
@@ -5076,7 +5076,7 @@
         <v>8</v>
       </c>
       <c r="E186" t="s" s="162">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F186" s="162"/>
     </row>
@@ -5900,7 +5900,7 @@
         <v>8</v>
       </c>
       <c r="E246" t="s" s="219">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F246" t="s" s="219">
         <v>193</v>
@@ -5920,7 +5920,7 @@
         <v>8</v>
       </c>
       <c r="E247" t="s" s="220">
-        <v>197</v>
+        <v>121</v>
       </c>
       <c r="F247" t="s" s="220">
         <v>51</v>
@@ -5932,7 +5932,7 @@
         <v>10.0</v>
       </c>
       <c r="C248" t="s" s="221">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D248" t="s" s="221">
         <v>31</v>
@@ -5944,19 +5944,19 @@
     </row>
     <row r="249">
       <c r="A249" t="s" s="222">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B249" t="n" s="222">
         <v>11.0</v>
       </c>
       <c r="C249" t="s" s="222">
+        <v>199</v>
+      </c>
+      <c r="D249" t="s" s="222">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s" s="222">
         <v>200</v>
-      </c>
-      <c r="D249" t="s" s="222">
-        <v>8</v>
-      </c>
-      <c r="E249" t="s" s="222">
-        <v>119</v>
       </c>
       <c r="F249" t="s" s="222">
         <v>201</v>
@@ -7710,7 +7710,7 @@
         <v>8</v>
       </c>
       <c r="E385" t="s" s="341">
-        <v>296</v>
+        <v>205</v>
       </c>
       <c r="F385" t="s" s="341">
         <v>42</v>
@@ -7724,13 +7724,13 @@
         <v>8.0</v>
       </c>
       <c r="C386" t="s" s="342">
+        <v>296</v>
+      </c>
+      <c r="D386" t="s" s="342">
+        <v>8</v>
+      </c>
+      <c r="E386" t="s" s="342">
         <v>297</v>
-      </c>
-      <c r="D386" t="s" s="342">
-        <v>8</v>
-      </c>
-      <c r="E386" t="s" s="342">
-        <v>298</v>
       </c>
       <c r="F386" t="s" s="342">
         <v>42</v>
@@ -7742,7 +7742,7 @@
         <v>9.0</v>
       </c>
       <c r="C387" t="s" s="343">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D387" t="s" s="343">
         <v>11</v>
@@ -7758,7 +7758,7 @@
         <v>10.0</v>
       </c>
       <c r="C388" t="s" s="344">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D388" t="s" s="344">
         <v>11</v>
@@ -7776,14 +7776,14 @@
         <v>11.0</v>
       </c>
       <c r="C389" t="s" s="345">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D389" t="s" s="345">
         <v>19</v>
       </c>
       <c r="E389" s="345"/>
       <c r="F389" t="s" s="345">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="390">
@@ -7792,7 +7792,7 @@
         <v>12.0</v>
       </c>
       <c r="C390" t="s" s="346">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D390" t="s" s="346">
         <v>19</v>
@@ -7806,7 +7806,7 @@
         <v>13.0</v>
       </c>
       <c r="C391" t="s" s="347">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D391" t="s" s="347">
         <v>19</v>
@@ -7820,7 +7820,7 @@
         <v>14.0</v>
       </c>
       <c r="C392" t="s" s="348">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D392" t="s" s="348">
         <v>19</v>
@@ -7836,13 +7836,13 @@
         <v>15.0</v>
       </c>
       <c r="C393" t="s" s="349">
+        <v>305</v>
+      </c>
+      <c r="D393" t="s" s="349">
+        <v>8</v>
+      </c>
+      <c r="E393" t="s" s="349">
         <v>306</v>
-      </c>
-      <c r="D393" t="s" s="349">
-        <v>8</v>
-      </c>
-      <c r="E393" t="s" s="349">
-        <v>307</v>
       </c>
       <c r="F393" s="349"/>
     </row>
@@ -7852,7 +7852,7 @@
         <v>16.0</v>
       </c>
       <c r="C394" t="s" s="350">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D394" t="s" s="350">
         <v>25</v>
@@ -7866,7 +7866,7 @@
         <v>17.0</v>
       </c>
       <c r="C395" t="s" s="351">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D395" t="s" s="351">
         <v>114</v>
@@ -7882,13 +7882,13 @@
         <v>18.0</v>
       </c>
       <c r="C396" t="s" s="352">
+        <v>309</v>
+      </c>
+      <c r="D396" t="s" s="352">
+        <v>8</v>
+      </c>
+      <c r="E396" t="s" s="352">
         <v>310</v>
-      </c>
-      <c r="D396" t="s" s="352">
-        <v>8</v>
-      </c>
-      <c r="E396" t="s" s="352">
-        <v>311</v>
       </c>
       <c r="F396" s="352"/>
     </row>
@@ -7906,7 +7906,7 @@
         <v>8</v>
       </c>
       <c r="E397" t="s" s="353">
-        <v>121</v>
+        <v>311</v>
       </c>
       <c r="F397" s="353"/>
     </row>
@@ -7924,7 +7924,7 @@
         <v>8</v>
       </c>
       <c r="E398" t="s" s="354">
-        <v>197</v>
+        <v>313</v>
       </c>
       <c r="F398" s="354"/>
     </row>
@@ -7936,13 +7936,13 @@
         <v>21.0</v>
       </c>
       <c r="C399" t="s" s="355">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D399" t="s" s="355">
         <v>8</v>
       </c>
       <c r="E399" t="s" s="355">
-        <v>221</v>
+        <v>315</v>
       </c>
       <c r="F399" s="355"/>
     </row>
@@ -7952,7 +7952,7 @@
         <v>22.0</v>
       </c>
       <c r="C400" t="s" s="356">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D400" t="s" s="356">
         <v>19</v>
@@ -7966,7 +7966,7 @@
         <v>23.0</v>
       </c>
       <c r="C401" t="s" s="357">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D401" t="s" s="357">
         <v>19</v>
@@ -7980,7 +7980,7 @@
         <v>24.0</v>
       </c>
       <c r="C402" t="s" s="358">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D402" t="s" s="358">
         <v>114</v>
@@ -7994,7 +7994,7 @@
         <v>25.0</v>
       </c>
       <c r="C403" t="s" s="359">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D403" t="s" s="359">
         <v>19</v>
@@ -8008,7 +8008,7 @@
         <v>26.0</v>
       </c>
       <c r="C404" t="s" s="360">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D404" t="s" s="360">
         <v>16</v>
@@ -8022,7 +8022,7 @@
         <v>27.0</v>
       </c>
       <c r="C405" t="s" s="361">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D405" t="s" s="361">
         <v>19</v>
@@ -8036,7 +8036,7 @@
         <v>28.0</v>
       </c>
       <c r="C406" t="s" s="362">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D406" t="s" s="362">
         <v>16</v>
@@ -8050,7 +8050,7 @@
         <v>29.0</v>
       </c>
       <c r="C407" t="s" s="363">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D407" t="s" s="363">
         <v>16</v>
@@ -8066,13 +8066,13 @@
         <v>30.0</v>
       </c>
       <c r="C408" t="s" s="364">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D408" t="s" s="364">
         <v>8</v>
       </c>
       <c r="E408" t="s" s="364">
-        <v>209</v>
+        <v>325</v>
       </c>
       <c r="F408" s="364"/>
     </row>
@@ -8082,7 +8082,7 @@
         <v>31.0</v>
       </c>
       <c r="C409" t="s" s="365">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D409" t="s" s="365">
         <v>8</v>
@@ -8096,7 +8096,7 @@
         <v>32.0</v>
       </c>
       <c r="C410" t="s" s="366">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D410" t="s" s="366">
         <v>19</v>
@@ -8112,7 +8112,7 @@
         <v>33.0</v>
       </c>
       <c r="C411" t="s" s="367">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D411" t="s" s="367">
         <v>19</v>
@@ -8184,7 +8184,7 @@
         <v>4.0</v>
       </c>
       <c r="C417" t="s" s="372">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D417" t="s" s="372">
         <v>16</v>
@@ -8282,7 +8282,7 @@
         <v>11.0</v>
       </c>
       <c r="C424" t="s" s="379">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D424" t="s" s="379">
         <v>8</v>
@@ -8296,7 +8296,7 @@
         <v>12.0</v>
       </c>
       <c r="C425" t="s" s="380">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D425" t="s" s="380">
         <v>11</v>
@@ -8310,7 +8310,7 @@
         <v>13.0</v>
       </c>
       <c r="C426" t="s" s="381">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D426" t="s" s="381">
         <v>11</v>
@@ -8324,7 +8324,7 @@
         <v>14.0</v>
       </c>
       <c r="C427" t="s" s="382">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D427" t="s" s="382">
         <v>19</v>
@@ -8338,7 +8338,7 @@
         <v>15.0</v>
       </c>
       <c r="C428" t="s" s="383">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D428" t="s" s="383">
         <v>19</v>
@@ -8352,7 +8352,7 @@
         <v>16.0</v>
       </c>
       <c r="C429" t="s" s="384">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D429" t="s" s="384">
         <v>19</v>
@@ -8366,7 +8366,7 @@
         <v>17.0</v>
       </c>
       <c r="C430" t="s" s="385">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D430" t="s" s="385">
         <v>19</v>
@@ -8380,7 +8380,7 @@
         <v>18.0</v>
       </c>
       <c r="C431" t="s" s="386">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D431" t="s" s="386">
         <v>8</v>
@@ -8394,7 +8394,7 @@
         <v>19.0</v>
       </c>
       <c r="C432" t="s" s="387">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D432" t="s" s="387">
         <v>25</v>
@@ -8408,7 +8408,7 @@
         <v>20.0</v>
       </c>
       <c r="C433" t="s" s="388">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D433" t="s" s="388">
         <v>114</v>
@@ -8422,7 +8422,7 @@
         <v>21.0</v>
       </c>
       <c r="C434" t="s" s="389">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D434" t="s" s="389">
         <v>8</v>
@@ -8464,7 +8464,7 @@
         <v>24.0</v>
       </c>
       <c r="C437" t="s" s="392">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D437" t="s" s="392">
         <v>8</v>
@@ -8478,7 +8478,7 @@
         <v>25.0</v>
       </c>
       <c r="C438" t="s" s="393">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D438" t="s" s="393">
         <v>19</v>
@@ -8492,7 +8492,7 @@
         <v>26.0</v>
       </c>
       <c r="C439" t="s" s="394">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D439" t="s" s="394">
         <v>19</v>
@@ -8506,7 +8506,7 @@
         <v>27.0</v>
       </c>
       <c r="C440" t="s" s="395">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D440" t="s" s="395">
         <v>114</v>
@@ -8520,7 +8520,7 @@
         <v>28.0</v>
       </c>
       <c r="C441" t="s" s="396">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D441" t="s" s="396">
         <v>19</v>
@@ -8534,7 +8534,7 @@
         <v>29.0</v>
       </c>
       <c r="C442" t="s" s="397">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D442" t="s" s="397">
         <v>16</v>
@@ -8548,7 +8548,7 @@
         <v>30.0</v>
       </c>
       <c r="C443" t="s" s="398">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D443" t="s" s="398">
         <v>19</v>
@@ -8562,7 +8562,7 @@
         <v>31.0</v>
       </c>
       <c r="C444" t="s" s="399">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D444" t="s" s="399">
         <v>16</v>
@@ -8576,7 +8576,7 @@
         <v>32.0</v>
       </c>
       <c r="C445" t="s" s="400">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D445" t="s" s="400">
         <v>16</v>
@@ -8590,7 +8590,7 @@
         <v>33.0</v>
       </c>
       <c r="C446" t="s" s="401">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D446" t="s" s="401">
         <v>8</v>
@@ -8604,7 +8604,7 @@
         <v>34.0</v>
       </c>
       <c r="C447" t="s" s="402">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D447" t="s" s="402">
         <v>8</v>
@@ -8618,7 +8618,7 @@
         <v>35.0</v>
       </c>
       <c r="C448" t="s" s="403">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D448" t="s" s="403">
         <v>19</v>
@@ -8632,7 +8632,7 @@
         <v>36.0</v>
       </c>
       <c r="C449" t="s" s="404">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D449" t="s" s="404">
         <v>19</v>
@@ -8656,7 +8656,7 @@
     </row>
     <row r="452">
       <c r="A452" s="406" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B452" s="406"/>
       <c r="C452" s="406"/>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="472">
       <c r="A472" s="424" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B472" s="424"/>
       <c r="C472" s="424"/>
@@ -9058,7 +9058,7 @@
     </row>
     <row r="484">
       <c r="A484" s="434" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B484" s="434"/>
       <c r="C484" s="434"/>
@@ -9226,7 +9226,7 @@
         <v>8</v>
       </c>
       <c r="E497" t="s" s="445">
-        <v>330</v>
+        <v>238</v>
       </c>
       <c r="F497" s="445"/>
     </row>
@@ -9238,13 +9238,13 @@
         <v>2.0</v>
       </c>
       <c r="C498" t="s" s="446">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D498" t="s" s="446">
         <v>8</v>
       </c>
       <c r="E498" t="s" s="446">
-        <v>238</v>
+        <v>334</v>
       </c>
       <c r="F498" s="446"/>
     </row>
@@ -9298,7 +9298,7 @@
         <v>3.0</v>
       </c>
       <c r="C503" t="s" s="450">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D503" t="s" s="450">
         <v>8</v>
@@ -9336,7 +9336,7 @@
         <v>8</v>
       </c>
       <c r="E505" t="s" s="452">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F505" s="452"/>
     </row>
@@ -9388,13 +9388,13 @@
         <v>2.0</v>
       </c>
       <c r="C510" t="s" s="456">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D510" t="s" s="456">
         <v>8</v>
       </c>
       <c r="E510" t="s" s="456">
-        <v>333</v>
+        <v>163</v>
       </c>
       <c r="F510" s="456"/>
     </row>
@@ -9412,7 +9412,7 @@
         <v>8</v>
       </c>
       <c r="E511" t="s" s="457">
-        <v>334</v>
+        <v>288</v>
       </c>
       <c r="F511" s="457"/>
     </row>
@@ -9580,7 +9580,7 @@
         <v>4.0</v>
       </c>
       <c r="C524" t="s" s="469">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D524" t="s" s="469">
         <v>8</v>
@@ -9760,7 +9760,7 @@
         <v>2.0</v>
       </c>
       <c r="C538" t="s" s="482">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D538" t="s" s="482">
         <v>19</v>
@@ -9778,13 +9778,13 @@
         <v>3.0</v>
       </c>
       <c r="C539" t="s" s="483">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D539" t="s" s="483">
         <v>8</v>
       </c>
       <c r="E539" t="s" s="483">
-        <v>333</v>
+        <v>163</v>
       </c>
       <c r="F539" s="483"/>
     </row>
@@ -9802,7 +9802,7 @@
         <v>8</v>
       </c>
       <c r="E540" t="s" s="484">
-        <v>334</v>
+        <v>288</v>
       </c>
       <c r="F540" s="484"/>
     </row>
@@ -9898,7 +9898,7 @@
         <v>6.0</v>
       </c>
       <c r="C548" t="s" s="491">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D548" t="s" s="491">
         <v>19</v>
@@ -9912,7 +9912,7 @@
         <v>7.0</v>
       </c>
       <c r="C549" t="s" s="492">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D549" t="s" s="492">
         <v>8</v>
@@ -9936,7 +9936,7 @@
     </row>
     <row r="552">
       <c r="A552" s="494" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B552" s="494"/>
       <c r="C552" s="494"/>
@@ -9966,7 +9966,7 @@
         <v>2.0</v>
       </c>
       <c r="C554" t="s" s="496">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D554" t="s" s="496">
         <v>31</v>
@@ -9980,7 +9980,7 @@
         <v>3.0</v>
       </c>
       <c r="C555" t="s" s="497">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D555" t="s" s="497">
         <v>31</v>
@@ -10008,7 +10008,7 @@
         <v>5.0</v>
       </c>
       <c r="C557" t="s" s="499">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D557" t="s" s="499">
         <v>31</v>
@@ -10022,7 +10022,7 @@
         <v>6.0</v>
       </c>
       <c r="C558" t="s" s="500">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D558" t="s" s="500">
         <v>114</v>
@@ -10032,7 +10032,7 @@
     </row>
     <row r="560">
       <c r="A560" s="501" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B560" s="501"/>
       <c r="C560" s="501"/>
@@ -10062,7 +10062,7 @@
         <v>2.0</v>
       </c>
       <c r="C562" t="s" s="503">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D562" t="s" s="503">
         <v>8</v>
@@ -10076,7 +10076,7 @@
         <v>3.0</v>
       </c>
       <c r="C563" t="s" s="504">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D563" t="s" s="504">
         <v>31</v>
@@ -10090,7 +10090,7 @@
         <v>4.0</v>
       </c>
       <c r="C564" t="s" s="505">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D564" t="s" s="505">
         <v>31</v>
@@ -10128,13 +10128,13 @@
     </row>
     <row r="568">
       <c r="A568" t="s" s="508">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B568" t="n" s="508">
         <v>2.0</v>
       </c>
       <c r="C568" t="s" s="508">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D568" t="s" s="508">
         <v>8</v>
@@ -10152,7 +10152,7 @@
         <v>3.0</v>
       </c>
       <c r="C569" t="s" s="509">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D569" t="s" s="509">
         <v>103</v>
@@ -10166,7 +10166,7 @@
         <v>4.0</v>
       </c>
       <c r="C570" t="s" s="510">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D570" t="s" s="510">
         <v>19</v>
@@ -10180,7 +10180,7 @@
         <v>5.0</v>
       </c>
       <c r="C571" t="s" s="511">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D571" t="s" s="511">
         <v>25</v>
@@ -10194,7 +10194,7 @@
         <v>6.0</v>
       </c>
       <c r="C572" t="s" s="512">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D572" t="s" s="512">
         <v>103</v>
@@ -10274,7 +10274,7 @@
         <v>8</v>
       </c>
       <c r="E578" t="s" s="517">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F578" s="517"/>
     </row>
@@ -10298,7 +10298,7 @@
         <v>6.0</v>
       </c>
       <c r="C580" t="s" s="519">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D580" t="s" s="519">
         <v>8</v>
@@ -10312,7 +10312,7 @@
         <v>7.0</v>
       </c>
       <c r="C581" t="s" s="520">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D581" t="s" s="520">
         <v>103</v>
@@ -10326,7 +10326,7 @@
         <v>8.0</v>
       </c>
       <c r="C582" t="s" s="521">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D582" t="s" s="521">
         <v>19</v>
@@ -10340,7 +10340,7 @@
         <v>9.0</v>
       </c>
       <c r="C583" t="s" s="522">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D583" t="s" s="522">
         <v>25</v>
@@ -10354,7 +10354,7 @@
         <v>10.0</v>
       </c>
       <c r="C584" t="s" s="523">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D584" t="s" s="523">
         <v>103</v>
@@ -10394,7 +10394,7 @@
         <v>2.0</v>
       </c>
       <c r="C588" t="s" s="526">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D588" t="s" s="526">
         <v>8</v>
@@ -10410,13 +10410,13 @@
         <v>3.0</v>
       </c>
       <c r="C589" t="s" s="527">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D589" t="s" s="527">
         <v>8</v>
       </c>
       <c r="E589" t="s" s="527">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F589" s="527"/>
     </row>
@@ -10426,13 +10426,13 @@
         <v>4.0</v>
       </c>
       <c r="C590" t="s" s="528">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D590" t="s" s="528">
         <v>150</v>
       </c>
       <c r="E590" t="s" s="528">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F590" s="528"/>
     </row>
@@ -10442,13 +10442,13 @@
         <v>5.0</v>
       </c>
       <c r="C591" t="s" s="529">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D591" t="s" s="529">
         <v>31</v>
       </c>
       <c r="E591" t="s" s="529">
-        <v>356</v>
+        <v>151</v>
       </c>
       <c r="F591" s="529"/>
     </row>
@@ -10530,7 +10530,7 @@
         <v>4.0</v>
       </c>
       <c r="C598" t="s" s="535">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D598" t="s" s="535">
         <v>8</v>
@@ -10544,7 +10544,7 @@
         <v>5.0</v>
       </c>
       <c r="C599" t="s" s="536">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D599" t="s" s="536">
         <v>11</v>
@@ -10558,7 +10558,7 @@
         <v>6.0</v>
       </c>
       <c r="C600" t="s" s="537">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D600" t="s" s="537">
         <v>8</v>
@@ -10572,7 +10572,7 @@
         <v>7.0</v>
       </c>
       <c r="C601" t="s" s="538">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D601" t="s" s="538">
         <v>31</v>
@@ -10800,7 +10800,7 @@
         <v>8</v>
       </c>
       <c r="E618" t="s" s="553">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F618" s="553"/>
     </row>
@@ -11423,7 +11423,7 @@
       </c>
       <c r="E670" s="597"/>
       <c r="F670" t="s" s="597">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="671">
@@ -11439,7 +11439,7 @@
       </c>
       <c r="E671" s="598"/>
       <c r="F671" t="s" s="598">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="672">
@@ -11451,7 +11451,7 @@
       <c r="D672" s="599"/>
       <c r="E672" s="599"/>
       <c r="F672" t="s" s="599">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="674">
@@ -11540,7 +11540,7 @@
         <v>8</v>
       </c>
       <c r="E680" t="s" s="605">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F680" s="605"/>
     </row>
@@ -11558,7 +11558,7 @@
         <v>8</v>
       </c>
       <c r="E681" t="s" s="606">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="F681" s="606"/>
     </row>
@@ -11688,7 +11688,7 @@
         <v>8</v>
       </c>
       <c r="E692" t="s" s="615">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F692" s="615"/>
     </row>
@@ -11722,7 +11722,7 @@
     </row>
     <row r="696">
       <c r="A696" s="618" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B696" s="618"/>
       <c r="C696" s="618"/>
@@ -11856,7 +11856,7 @@
         <v>9.0</v>
       </c>
       <c r="C705" t="s" s="627">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D705" t="s" s="627">
         <v>19</v>
@@ -12048,7 +12048,7 @@
         <v>8</v>
       </c>
       <c r="E720" t="s" s="640">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F720" s="640"/>
     </row>
@@ -12124,7 +12124,7 @@
         <v>8</v>
       </c>
       <c r="E726" t="s" s="645">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F726" s="645"/>
     </row>
@@ -12376,7 +12376,7 @@
         <v>8</v>
       </c>
       <c r="E745" t="s" s="663">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F745" s="663"/>
     </row>
@@ -12394,7 +12394,7 @@
         <v>8</v>
       </c>
       <c r="E746" t="s" s="664">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="F746" s="664"/>
     </row>
@@ -12672,7 +12672,7 @@
         <v>8</v>
       </c>
       <c r="E768" t="s" s="683">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F768" s="683"/>
     </row>

</xml_diff>